<commit_message>
Update ERD and DD
Removed inventroy_id from Item table, edit constraints
</commit_message>
<xml_diff>
--- a/Group_2_DD_DD.xlsx
+++ b/Group_2_DD_DD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denis.DESKTOP-PCM19BM\Desktop\doomsday-prep-group-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F77FBDD-CB4A-4B8C-8D88-F44A79536FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D24B823-8926-4194-A8A7-1A1F5ECF1E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32310" yWindow="1080" windowWidth="21600" windowHeight="14535" xr2:uid="{90F0B15E-D7D7-4F06-BF48-AC0E0024389C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{90F0B15E-D7D7-4F06-BF48-AC0E0024389C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="154">
   <si>
     <t>Attribute</t>
   </si>
@@ -137,9 +137,6 @@
     <t>item_id</t>
   </si>
   <si>
-    <t>inventory_id</t>
-  </si>
-  <si>
     <t>item_name</t>
   </si>
   <si>
@@ -257,12 +254,6 @@
     <t>status_name</t>
   </si>
   <si>
-    <t>what was changed</t>
-  </si>
-  <si>
-    <t>need to remove</t>
-  </si>
-  <si>
     <t>Unique identifier for the city.</t>
   </si>
   <si>
@@ -344,9 +335,6 @@
     <t>Unique identifier for the item.</t>
   </si>
   <si>
-    <t>Identifier of the inventory where the item is stored.</t>
-  </si>
-  <si>
     <t>Name of the item.</t>
   </si>
   <si>
@@ -356,9 +344,6 @@
     <t>Indicates whether the item is used as currency.</t>
   </si>
   <si>
-    <t>read comment</t>
-  </si>
-  <si>
     <t>Value of a single unit of the item.</t>
   </si>
   <si>
@@ -446,9 +431,6 @@
     <t>Identifier of the faction involved.</t>
   </si>
   <si>
-    <t>All comments and fill colors will be removed before submission.</t>
-  </si>
-  <si>
     <t>state</t>
   </si>
   <si>
@@ -510,13 +492,19 @@
   </si>
   <si>
     <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>NOT NULL DEFAULT 1</t>
+  </si>
+  <si>
+    <t>NOT NULL DEFAULT 0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -539,31 +527,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -658,37 +633,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1023,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD9435C-6168-4176-834E-32B2C91F608A}">
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,1221 +1016,1241 @@
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
     <col min="6" max="6" width="61.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="4"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" s="9"/>
-      <c r="I3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" t="s">
-        <v>62</v>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
       <c r="F4" s="13" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E5" t="s">
-        <v>156</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="E5" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" t="s">
-        <v>157</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="C7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="11"/>
-      <c r="F7" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="C8" t="s">
-        <v>61</v>
+    <row r="8" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="D8" s="11"/>
-      <c r="E8" t="s">
-        <v>157</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="C9" t="s">
-        <v>61</v>
+      <c r="E8" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="D9" s="11"/>
-      <c r="E9" t="s">
-        <v>157</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="E9" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E10" t="s">
-        <v>156</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="E10" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
       <c r="B11" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" t="s">
-        <v>157</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="C12" t="s">
-        <v>63</v>
-      </c>
       <c r="D12" s="11"/>
-      <c r="F12" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="C13" t="s">
-        <v>62</v>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="D13" s="11"/>
-      <c r="E13" t="s">
-        <v>157</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="E13" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E14" t="s">
-        <v>156</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="E14" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
       <c r="B15" s="11" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E15" t="s">
-        <v>157</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="E15" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" t="s">
-        <v>62</v>
+        <v>68</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="D16" s="11"/>
-      <c r="E16" t="s">
-        <v>157</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>83</v>
+      <c r="E16" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" s="11"/>
-      <c r="F17" s="5" t="s">
-        <v>84</v>
+      <c r="E17" s="12"/>
+      <c r="F17" s="13" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E18" t="s">
-        <v>156</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>85</v>
+      <c r="E18" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E19" t="s">
-        <v>157</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>86</v>
+      <c r="E19" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
-        <v>62</v>
+      <c r="C20" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="D20" s="11"/>
-      <c r="E20" t="s">
-        <v>157</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>87</v>
+      <c r="E20" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
-        <v>62</v>
+      <c r="C21" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="D21" s="11"/>
-      <c r="E21" t="s">
-        <v>157</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>88</v>
+      <c r="E21" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="11"/>
-      <c r="F22" s="5" t="s">
-        <v>89</v>
+      <c r="E22" s="12"/>
+      <c r="F22" s="13" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>90</v>
+      <c r="E23" s="12"/>
+      <c r="F23" s="13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E24" t="s">
-        <v>156</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>91</v>
+      <c r="E24" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" t="s">
-        <v>157</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="C26" t="s">
-        <v>63</v>
-      </c>
       <c r="D26" s="11"/>
-      <c r="F26" s="5" t="s">
-        <v>93</v>
+      <c r="E26" s="12"/>
+      <c r="F26" s="13" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E27" t="s">
-        <v>157</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>94</v>
+      <c r="E27" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E28" t="s">
-        <v>157</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>95</v>
+      <c r="E28" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
+      <c r="A29" s="10"/>
       <c r="B29" s="11" t="s">
         <v>26</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29" s="11"/>
-      <c r="F29" s="5" t="s">
-        <v>96</v>
+      <c r="E29" s="12"/>
+      <c r="F29" s="13" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E30" t="s">
-        <v>156</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>97</v>
+      <c r="E30" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E31" t="s">
-        <v>157</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>98</v>
+      <c r="E31" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
+      <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D32" s="11"/>
-      <c r="E32" t="s">
-        <v>157</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>99</v>
+      <c r="E32" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D33" s="11"/>
-      <c r="F33" s="5" t="s">
-        <v>100</v>
+      <c r="E33" s="12"/>
+      <c r="F33" s="13" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>32</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E34" t="s">
-        <v>156</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>101</v>
+      <c r="E34" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>102</v>
+      <c r="C35" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="11"/>
+      <c r="E35" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C36" t="s">
-        <v>62</v>
+      <c r="C36" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="D36" s="11"/>
-      <c r="E36" t="s">
-        <v>157</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>103</v>
+      <c r="E36" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C37" t="s">
-        <v>62</v>
+      <c r="C37" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="D37" s="11"/>
-      <c r="E37" t="s">
-        <v>157</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>104</v>
+      <c r="E37" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="11"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D38" s="11"/>
-      <c r="F38" s="5" t="s">
+      <c r="D41" s="11"/>
+      <c r="E41" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F41" s="13" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
-      <c r="B39" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C39" t="s">
-        <v>65</v>
-      </c>
-      <c r="D39" s="11"/>
-      <c r="F39" s="5" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" s="11"/>
+      <c r="E42" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D43" s="11"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="13" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C40" s="11" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+      <c r="B44" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D44" s="11"/>
+      <c r="E44" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E40" t="s">
-        <v>156</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
-      <c r="B41" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="F41" s="5" t="s">
+      <c r="E45" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F45" s="13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
-      <c r="B42" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" t="s">
-        <v>62</v>
-      </c>
-      <c r="D42" s="11"/>
-      <c r="E42" t="s">
-        <v>157</v>
-      </c>
-      <c r="F42" s="5" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" s="11"/>
+      <c r="E46" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F46" s="13" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
-      <c r="B43" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="C43" t="s">
-        <v>62</v>
-      </c>
-      <c r="D43" s="11"/>
-      <c r="E43" t="s">
-        <v>157</v>
-      </c>
-      <c r="F43" s="5" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="B47" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="11"/>
+      <c r="E47" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F47" s="13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
-      <c r="B44" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C44" t="s">
-        <v>63</v>
-      </c>
-      <c r="D44" s="11"/>
-      <c r="F44" s="5" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="B48" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" s="11"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="13" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
-      <c r="B45" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D45" s="11"/>
-      <c r="F45" s="5" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F49" s="13" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" t="s">
-        <v>156</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
-      <c r="B47" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C47" t="s">
-        <v>62</v>
-      </c>
-      <c r="D47" s="11"/>
-      <c r="E47" t="s">
-        <v>157</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="16"/>
-      <c r="B48" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" t="s">
-        <v>62</v>
-      </c>
-      <c r="D48" s="11"/>
-      <c r="E48" t="s">
-        <v>157</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
-      <c r="B49" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C49" t="s">
-        <v>62</v>
-      </c>
-      <c r="D49" s="11"/>
-      <c r="F49" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
-        <v>46</v>
-      </c>
+      <c r="A50" s="10"/>
       <c r="B50" s="11" t="s">
         <v>47</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D50" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" t="s">
-        <v>156</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>118</v>
+        <v>63</v>
+      </c>
+      <c r="D50" s="11"/>
+      <c r="E50" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F50" s="13" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
+      <c r="A51" s="10"/>
       <c r="B51" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="11" t="s">
-        <v>64</v>
+      <c r="C51" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="D51" s="11"/>
-      <c r="E51" t="s">
-        <v>157</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>119</v>
+      <c r="E51" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
+      <c r="A52" s="10"/>
       <c r="B52" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D52" s="11"/>
+      <c r="E52" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="B53" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D53" s="11"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C52" t="s">
-        <v>62</v>
-      </c>
-      <c r="D52" s="11"/>
-      <c r="E52" t="s">
-        <v>157</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
-      <c r="B53" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="C53" t="s">
-        <v>62</v>
-      </c>
-      <c r="D53" s="11"/>
-      <c r="E53" t="s">
-        <v>157</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
-      <c r="B54" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="C54" t="s">
-        <v>63</v>
-      </c>
-      <c r="D54" s="11"/>
-      <c r="F54" s="5" t="s">
-        <v>121</v>
+      <c r="B54" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
-        <v>50</v>
-      </c>
+      <c r="A55" s="10"/>
       <c r="B55" s="11" t="s">
         <v>51</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D55" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E55" t="s">
-        <v>157</v>
-      </c>
-      <c r="F55" s="5" t="s">
+      <c r="E55" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+      <c r="B56" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D56" s="11"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="10"/>
+      <c r="B58" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D58" s="11"/>
+      <c r="E58" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F59" s="13" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
-      <c r="B56" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E56" t="s">
-        <v>157</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
-      <c r="B57" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C57" t="s">
-        <v>62</v>
-      </c>
-      <c r="D57" s="11"/>
-      <c r="F57" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C58" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E58" t="s">
-        <v>156</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="16"/>
-      <c r="B59" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C59" t="s">
-        <v>62</v>
-      </c>
-      <c r="D59" s="11"/>
-      <c r="E59" t="s">
-        <v>157</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
-        <v>54</v>
-      </c>
+      <c r="A60" s="10"/>
       <c r="B60" s="11" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D60" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E60" t="s">
-        <v>157</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>127</v>
+      <c r="E60" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F60" s="13" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="16"/>
+      <c r="A61" s="10"/>
       <c r="B61" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D61" s="11"/>
+      <c r="E61" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F61" s="13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B62" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D61" s="11" t="s">
+      <c r="C62" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D62" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E61" t="s">
-        <v>157</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="16"/>
-      <c r="B62" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D62" s="11"/>
-      <c r="E62" t="s">
-        <v>157</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>129</v>
+      <c r="E62" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F62" s="13" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
-        <v>56</v>
-      </c>
+      <c r="A63" s="10"/>
       <c r="B63" s="11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D63" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E63" t="s">
-        <v>157</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>130</v>
+      <c r="E63" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F63" s="13" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="16"/>
+      <c r="A64" s="10" t="s">
+        <v>56</v>
+      </c>
       <c r="B64" s="11" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D64" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E64" t="s">
-        <v>157</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>131</v>
+      <c r="E64" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="16" t="s">
-        <v>57</v>
-      </c>
+      <c r="A65" s="10"/>
       <c r="B65" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D65" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E65" t="s">
-        <v>157</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>130</v>
+      <c r="E65" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F65" s="13" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="16"/>
+      <c r="A66" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="B66" s="11" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D66" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E66" t="s">
-        <v>157</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>132</v>
+      <c r="E66" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F66" s="13" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="16" t="s">
-        <v>58</v>
-      </c>
+      <c r="A67" s="10"/>
       <c r="B67" s="11" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D67" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E67" t="s">
-        <v>157</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>133</v>
+      <c r="E67" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F67" s="13" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="16"/>
+      <c r="A68" s="10" t="s">
+        <v>58</v>
+      </c>
       <c r="B68" s="11" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D68" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E68" t="s">
-        <v>157</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C69" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D69" s="11" t="s">
+      <c r="E68" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F68" s="13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="17"/>
+      <c r="B69" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D69" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E69" t="s">
-        <v>157</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="17"/>
-      <c r="B70" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C70" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D70" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E70" t="s">
-        <v>157</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>135</v>
+      <c r="E69" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="F69" s="20" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A49:A53"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="A18:A23"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A34:A39"/>
-    <mergeCell ref="A40:A45"/>
-    <mergeCell ref="A46:A49"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="A45:A48"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="A66:A67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>